<commit_message>
corrected negative values in ABDa2009;implemented metal-oxide consolidation functions
</commit_message>
<xml_diff>
--- a/input_data/ABD2009a.xlsx
+++ b/input_data/ABD2009a.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rui/Harvard Drive/Readings/Archaeology/Glass/Data/input_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E3EB6F9-A2DC-3E47-8616-97F542E02F6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{370C4141-03B1-2442-BE28-B81298DCF2BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15740" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="publication_information" sheetId="1" r:id="rId1"/>
@@ -494,7 +494,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1816,7 +1816,7 @@
   <dimension ref="A1:R17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1910,7 +1910,7 @@
         <v>0.05</v>
       </c>
       <c r="J3">
-        <v>-0.01</v>
+        <v>0.01</v>
       </c>
       <c r="K3">
         <v>1.24</v>
@@ -1939,7 +1939,7 @@
         <v>0.76</v>
       </c>
       <c r="J4">
-        <v>-0.02</v>
+        <v>0.02</v>
       </c>
       <c r="K4">
         <v>2.35</v>
@@ -2081,7 +2081,7 @@
         <v>0.05</v>
       </c>
       <c r="J9">
-        <v>-0.72</v>
+        <v>0.72</v>
       </c>
       <c r="K9">
         <v>2.5299999999999998</v>
@@ -2110,7 +2110,7 @@
         <v>0.05</v>
       </c>
       <c r="J10">
-        <v>-0.69</v>
+        <v>0.69</v>
       </c>
       <c r="K10">
         <v>2.4</v>
@@ -2139,7 +2139,7 @@
         <v>0.04</v>
       </c>
       <c r="J11">
-        <v>-0.03</v>
+        <v>0.03</v>
       </c>
       <c r="K11">
         <v>4.13</v>
@@ -2284,7 +2284,7 @@
         <v>2.73</v>
       </c>
       <c r="J16">
-        <v>-0.01</v>
+        <v>0.01</v>
       </c>
       <c r="K16">
         <v>2.38</v>
@@ -2313,7 +2313,7 @@
         <v>0.4</v>
       </c>
       <c r="J17">
-        <v>-0.02</v>
+        <v>0.02</v>
       </c>
       <c r="K17">
         <v>3.94</v>

</xml_diff>